<commit_message>
Proyecto Final - Regresión Lista
</commit_message>
<xml_diff>
--- a/Proyecto/Experimentos.xlsx
+++ b/Proyecto/Experimentos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos\Educación\Posgrado\Universidad Galileo (UG)\Trimestre II\Statistical Learning I\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEC36CC-1804-4DE9-88BA-1662CA9686EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B1E273-212C-441C-95A3-7BD3B6DC6CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{417B3B53-26E6-42C2-9D6A-9E900F281E7D}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{417B3B53-26E6-42C2-9D6A-9E900F281E7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Decision Tree" sheetId="1" r:id="rId1"/>
     <sheet name="SVM" sheetId="2" r:id="rId2"/>
+    <sheet name="Linear Regression" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
   <si>
     <t>ID Prueba</t>
   </si>
@@ -1279,6 +1280,54 @@
   </si>
   <si>
     <t>ACCURACY FINAL TEST: 0.7973</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Batch Size</t>
+  </si>
+  <si>
+    <t>["age_norm", "sibsp_norm", "parch_norm", "fare_per_person_norm", "C", "Q", "S", "passenger_class", "passenger_sex", "last_name", "honorific", "ticket_prefix", "ticket_number_norm", "married", "survived"]</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>La accuracy es igual a 1 porque esta aún se encontraba oscilando y en una de las oscilaciones alcanzó una precisión de 1. Probablemente un caso de overfit</t>
+  </si>
+  <si>
+    <t>Nuevamente la precisión comenzó a oscilar y se detuvo en 1. Overfit seguro</t>
+  </si>
+  <si>
+    <t>La accuracy dejó de oscilar tanto, pero el proceso necesita más epochs para mejorar los resultados</t>
+  </si>
+  <si>
+    <t>Aquí se vio que el modelo todavía tiene bastante que mejorar si se aumenta el tiempo de entrenamiento. Se va a bajar el lr para acelerar el proceso</t>
+  </si>
+  <si>
+    <t>Mejoró sustancialmente. Se bajará nuevamente el learning rate</t>
+  </si>
+  <si>
+    <t>Se va a extender el tiempo de entrenamiento para ver si se estabiliza el proceso de entrenamiento</t>
+  </si>
+  <si>
+    <t>Se estabilizó el entrenamiento. Parece que este es el valor más pequeño de error que puede ser obtenido</t>
+  </si>
+  <si>
+    <t>Parece que el efecto de incrementar el batch size es "suavizar" o estabilizar los gráficos de las métricas (reduce varianza)</t>
+  </si>
+  <si>
+    <t>Se eligirá este modelo porque parece haberse estabilizado en su desempeño</t>
+  </si>
+  <si>
+    <t>ACCURACY FINAL TEST: 0.8018</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1450,6 +1499,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1458,6 +1510,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2045,12 +2103,12 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="24" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="25" t="s">
         <v>75</v>
       </c>
       <c r="G13" s="1"/>
@@ -2243,7 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF2ACC6-038A-47B6-9458-956964B62FE2}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
@@ -3205,15 +3263,15 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="24" t="s">
+      <c r="A34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="25" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3246,4 +3304,350 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584C84FB-AD93-431F-8EA9-286C0CCA33E9}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="75.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="49.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="11">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="11">
+        <v>32</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.29930000000000001</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="11">
+        <v>64</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.61919999999999997</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="D6" s="11">
+        <v>2000</v>
+      </c>
+      <c r="E6" s="11">
+        <v>64</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.63639999999999997</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1E-3</v>
+      </c>
+      <c r="D7" s="11">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="11">
+        <v>64</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.3972</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.87880000000000003</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2000</v>
+      </c>
+      <c r="E8" s="11">
+        <v>64</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.2213</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.90910000000000002</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3000</v>
+      </c>
+      <c r="E9" s="11">
+        <v>64</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.20710000000000001</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.90910000000000002</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="11">
+        <v>3000</v>
+      </c>
+      <c r="E10" s="11">
+        <v>128</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.34720000000000001</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="11">
+        <v>4000</v>
+      </c>
+      <c r="E11" s="11">
+        <v>128</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.34489999999999998</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="20">
+        <v>6000</v>
+      </c>
+      <c r="E12" s="20">
+        <v>128</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="G12" s="19">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Proyecto Final - Deployment Listo
</commit_message>
<xml_diff>
--- a/Proyecto/Experimentos.xlsx
+++ b/Proyecto/Experimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos\Educación\Posgrado\Universidad Galileo (UG)\Trimestre II\Statistical Learning I\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B1E273-212C-441C-95A3-7BD3B6DC6CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA6C99A-4AC9-462E-9C06-67EF40BC0F14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{417B3B53-26E6-42C2-9D6A-9E900F281E7D}"/>
   </bookViews>
@@ -1469,21 +1469,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1515,6 +1500,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1847,36 +1847,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
@@ -2079,36 +2079,36 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="14">
         <v>0.82799999999999996</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="14">
         <v>0.80700000000000005</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="17" t="s">
         <v>73</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="25" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="20" t="s">
         <v>75</v>
       </c>
       <c r="G13" s="1"/>
@@ -2301,7 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF2ACC6-038A-47B6-9458-956964B62FE2}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
@@ -2319,46 +2319,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="27" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -2825,34 +2825,34 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="14">
         <v>17</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="15">
         <v>3</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="15">
         <v>2</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="15">
         <v>0.1</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="16">
         <v>0</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="14">
         <v>0.86990000000000001</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="14">
         <v>0.82840000000000003</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="17" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3263,15 +3263,15 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="25" t="s">
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="20" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3328,48 +3328,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="27" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C3" s="11">
@@ -3395,7 +3395,7 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="11">
@@ -3421,7 +3421,7 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="11">
@@ -3447,7 +3447,7 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="11">
@@ -3473,7 +3473,7 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C7" s="11">
@@ -3499,7 +3499,7 @@
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C8" s="11">
@@ -3517,7 +3517,7 @@
       <c r="G8" s="3">
         <v>0.90910000000000002</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="19" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="11">
@@ -3551,7 +3551,7 @@
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="11">
@@ -3577,7 +3577,7 @@
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C11" s="11">
@@ -3598,43 +3598,43 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="15">
         <v>0.01</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="15">
         <v>6000</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="15">
         <v>128</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="14">
         <v>0.34250000000000003</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="14">
         <v>0.86599999999999999</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="17" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="25" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="20" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>